<commit_message>
update for release 1.048
</commit_message>
<xml_diff>
--- a/manifest.xlsx
+++ b/manifest.xlsx
@@ -103,34 +103,34 @@
     <t>p3_core</t>
   </si>
   <si>
+    <t>2025-08-06T20:32:44Z</t>
+  </si>
+  <si>
+    <t>olsonanl:75 bparrello:39 JacobPorter:3</t>
+  </si>
+  <si>
+    <t>p3_deployment</t>
+  </si>
+  <si>
+    <t>2024-06-28T21:29:48Z</t>
+  </si>
+  <si>
+    <t>olsonanl:6</t>
+  </si>
+  <si>
+    <t>sars2_assembly</t>
+  </si>
+  <si>
+    <t>2024-06-28T22:29:40Z</t>
+  </si>
+  <si>
+    <t>olsonanl:106 aswarren:2 nicolegobo:1</t>
+  </si>
+  <si>
+    <t>seed_core</t>
+  </si>
+  <si>
     <t>Robert Olson</t>
-  </si>
-  <si>
-    <t>2025-05-07T17:39:36Z</t>
-  </si>
-  <si>
-    <t>olsonanl:74 bparrello:24 JacobPorter:3</t>
-  </si>
-  <si>
-    <t>p3_deployment</t>
-  </si>
-  <si>
-    <t>2024-06-28T21:29:48Z</t>
-  </si>
-  <si>
-    <t>olsonanl:6</t>
-  </si>
-  <si>
-    <t>sars2_assembly</t>
-  </si>
-  <si>
-    <t>2024-06-28T22:29:40Z</t>
-  </si>
-  <si>
-    <t>olsonanl:106 aswarren:2 nicolegobo:1</t>
-  </si>
-  <si>
-    <t>seed_core</t>
   </si>
   <si>
     <t>2024-06-28T19:35:26Z</t>
@@ -695,22 +695,22 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>HYPERLINK("https://github.com/BV-BRC/p3_core/commit/af437528ced4432168cab95af78cd442b5834412", "af437528ced4432168cab95af78cd442b5834412")</f>
+        <f>HYPERLINK("https://github.com/BV-BRC/p3_core/commit/e6aed994a30ee0dd72784118c164ebe3ff2124a0", "e6aed994a30ee0dd72784118c164ebe3ff2124a0")</f>
         <v>0</v>
       </c>
       <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -727,15 +727,15 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
         <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -752,15 +752,15 @@
         <v>13</v>
       </c>
       <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
         <v>36</v>
-      </c>
-      <c r="G10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -774,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
         <v>42</v>
@@ -824,7 +824,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
         <v>45</v>

</xml_diff>